<commit_message>
Missing file in radiant.
</commit_message>
<xml_diff>
--- a/pcb/rev1/vera-module bom.xlsx
+++ b/pcb/rev1/vera-module bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\vera-module\pcb\rev1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{78DC8CD0-7479-4DB4-8FF0-385A2E4436B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEE9DE2-A36C-470C-99A5-BFA19177C07E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-11970" yWindow="4320" windowWidth="21600" windowHeight="11205"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vera-module bom" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -830,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -857,6 +857,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1213,23 +1220,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>4</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -1314,7 +1321,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -1365,7 +1372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>3</v>
       </c>
@@ -1382,7 +1389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1399,109 +1406,109 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+    <row r="12" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>3</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="13">
         <v>75</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+    <row r="13" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>3</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="13">
         <v>536</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+    <row r="14" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>3</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="13">
         <v>1070</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+    <row r="15" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>3</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="13">
         <v>2150</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+    <row r="16" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
         <v>3</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="13">
         <v>4300</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+    <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
         <v>9</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>1</v>
       </c>
@@ -1518,24 +1525,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+    <row r="20" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>2</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>15</v>
       </c>
@@ -1552,7 +1559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>2</v>
       </c>
@@ -1569,211 +1576,211 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="10" t="s">
+    <row r="23" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>1</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+    <row r="24" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>7</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+    <row r="25" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
         <v>5</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
-        <v>1</v>
-      </c>
-      <c r="B27" s="10" t="s">
+    <row r="27" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>1</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
-        <v>1</v>
-      </c>
-      <c r="B29" s="10" t="s">
+    <row r="29" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>1</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
-        <v>1</v>
-      </c>
-      <c r="B30" s="10" t="s">
+    <row r="30" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>1</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
-        <v>1</v>
-      </c>
-      <c r="B31" s="10" t="s">
+    <row r="31" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>1</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
-        <v>1</v>
-      </c>
-      <c r="B32" s="10" t="s">
+    <row r="32" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>1</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
-        <v>1</v>
-      </c>
-      <c r="B33" s="10" t="s">
+    <row r="33" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>1</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
-        <v>1</v>
-      </c>
-      <c r="B34" s="10" t="s">
+    <row r="34" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>1</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
-        <v>1</v>
-      </c>
-      <c r="B35" s="10" t="s">
+    <row r="35" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>1</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
-        <v>1</v>
-      </c>
-      <c r="B36" s="10" t="s">
+    <row r="36" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>1</v>
+      </c>
+      <c r="B36" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>1</v>
       </c>
@@ -1790,173 +1797,173 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
-        <v>1</v>
-      </c>
-      <c r="B39" s="10" t="s">
+    <row r="39" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>1</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
-        <v>1</v>
-      </c>
-      <c r="B40" s="10" t="s">
+    <row r="40" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>1</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
-        <v>1</v>
-      </c>
-      <c r="B41" s="10" t="s">
+    <row r="41" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>1</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9">
-        <v>1</v>
-      </c>
-      <c r="B42" s="10" t="s">
+    <row r="42" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <v>1</v>
+      </c>
+      <c r="B42" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9">
-        <v>1</v>
-      </c>
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <v>1</v>
+      </c>
+      <c r="B43" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9">
-        <v>1</v>
-      </c>
-      <c r="B44" s="10" t="s">
+    <row r="44" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <v>1</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9">
-        <v>1</v>
-      </c>
-      <c r="B45" s="10" t="s">
+    <row r="45" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
+        <v>1</v>
+      </c>
+      <c r="B45" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9">
-        <v>1</v>
-      </c>
-      <c r="B46" s="10" t="s">
+    <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12">
+        <v>1</v>
+      </c>
+      <c r="B46" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9">
-        <v>1</v>
-      </c>
-      <c r="B47" s="10" t="s">
+    <row r="47" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <v>1</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
+    <row r="48" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
         <v>3</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="12" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>